<commit_message>
fixed logout button in the banner
</commit_message>
<xml_diff>
--- a/Facilities.xlsx
+++ b/Facilities.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawabar/SD/Java/MidtermProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DBF9047-7910-AE49-AF0F-B8EFF1A2E037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50F49CC-7C8B-5C47-A219-21F16B57C973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32740" yWindow="2800" windowWidth="33600" windowHeight="20500" xr2:uid="{28F1DD02-C953-A74E-8E9A-0D6CED1E4C53}"/>
+    <workbookView xWindow="32000" yWindow="-1860" windowWidth="33600" windowHeight="21000" xr2:uid="{28F1DD02-C953-A74E-8E9A-0D6CED1E4C53}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DANCE" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>

</xml_diff>